<commit_message>
add henan hebei 2/13 0-24
</commit_message>
<xml_diff>
--- a/data/unchecked/manual_collect/china/henan/henanCaseStatistics_20200210.xlsx
+++ b/data/unchecked/manual_collect/china/henan/henanCaseStatistics_20200210.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22607"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\yiqing\pkuvis.github.io\NCP\data\unchecked\manual_collect\china\henan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\yiqing\COVID-19\data\unchecked\manual_collect\china\henan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3F914B-68ED-44AD-936B-5A0352ECFA71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99074BB3-9703-4B6F-ADD4-923732A3A555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,7 +1103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
       <selection activeCell="S176" sqref="S176:AF178"/>
     </sheetView>
   </sheetViews>

</xml_diff>